<commit_message>
added speaker boxes dir, crossover simulation
</commit_message>
<xml_diff>
--- a/Measurements/Filter Measurements(PCB).xlsx
+++ b/Measurements/Filter Measurements(PCB).xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -52,7 +52,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -823,27 +822,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2093927672"/>
-        <c:axId val="2092990328"/>
+        <c:axId val="2073478344"/>
+        <c:axId val="2073481336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2093927672"/>
+        <c:axId val="2073478344"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092990328"/>
+        <c:crossAx val="2073481336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2092990328"/>
+        <c:axId val="2073481336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093927672"/>
+        <c:crossAx val="2073478344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -880,16 +881,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2313,7 +2314,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>